<commit_message>
Product development plan Gantt chart
</commit_message>
<xml_diff>
--- a/Product development plan Gantt chart.xlsx
+++ b/Product development plan Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\startup_launch_simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BDF2EB-328A-40E2-B29B-3CD2134EC423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E993F28D-47D3-4A86-8947-C26F026D1DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6019ACCF-C646-4342-801A-80DB9B3D6D79}"/>
   </bookViews>
@@ -136,51 +136,341 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="waterfall" uniqueId="{D331B955-49B5-4CE7-B247-D6F3BD219864}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
-              <cx:v>End Date</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataLabels pos="outEnd">
-            <cx:visibility seriesName="0" categoryName="0" value="1"/>
-          </cx:dataLabels>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:subtotals/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0.5"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
-  </cx:chart>
-</cx:chartSpace>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="sr-Latn-RS"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration (Weeks)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>List1!$A$2:$B$8</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="7"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>01-10-25</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>16-10-25</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>01-11-25</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>16-12-25</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>06-01-26</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>27-01-26</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11-02-26</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Analiza zahtjeva i planiranje</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dizajn korisničkog interfejsa</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Razvoj backend i frontend</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Integracija plaćanja i sigurnosti</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Testiranje i kontrola kvaliteta</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Lansiranje pilot verzije</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Feedback i unapređenja</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1885-46CD-83F2-995744DB7B2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="561412464"/>
+        <c:axId val="561404304"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="561412464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561404304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="561404304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561412464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -224,7 +514,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="395">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -235,7 +525,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -258,7 +548,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -281,7 +571,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -289,11 +579,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -318,46 +608,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -372,8 +652,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -381,12 +663,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -396,13 +675,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -421,16 +700,18 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -501,6 +782,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -532,8 +819,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -588,7 +875,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -616,18 +903,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -637,9 +913,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -655,7 +934,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -671,7 +950,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -685,7 +964,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -718,7 +997,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -727,6 +1006,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -738,77 +1023,35 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1630680</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Grafikon 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB7CC6D8-77F6-B02A-007B-4CB5D7347F78}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="1482090"/>
-              <a:ext cx="7277100" cy="2800350"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>Ovaj grafikon nije dostupan u vašoj verziji programa Excel.
-Uređivanje ovog oblika ili čuvanje ove radne sveske u drugom formatu datoteke trajno će oštetiti grafikon.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafikon 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1643793E-9C8F-744B-F7CC-C12EA5FB1DF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1134,7 +1377,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:D8"/>
+      <selection activeCell="C1" activeCellId="2" sqref="A1:A1048576 B1:B1048576 C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,10 +1502,6 @@
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2">
-        <f>-E6</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>